<commit_message>
Atualizacoes manual e backlog
</commit_message>
<xml_diff>
--- a/documentos/Backlog.xlsx
+++ b/documentos/Backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="263">
   <si>
     <t>O sistema deverá ter um cadastro de Clientes com as seguintes opções: Inclusão, Alteração, Exclusão e Importação.</t>
   </si>
@@ -1186,7 +1186,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,11 +1203,11 @@
       </c>
       <c r="B1" s="2">
         <f>SUBTOTAL(3,B3:B26)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6">
         <f>B1/(A1)</f>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1296,6 +1296,9 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>